<commit_message>
Data of the coupled networks of Test System 1
</commit_message>
<xml_diff>
--- a/2.1. test system 1.xlsx
+++ b/2.1. test system 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AppData\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\GithubClone\supplementary-file-for-low-carbon-scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B621450-CB66-4582-862F-A70A133963D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9D023A-0046-4A40-B993-9252D64AC6EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="35216" windowHeight="19203" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TN params" sheetId="1" r:id="rId1"/>
@@ -190,20 +190,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -491,23 +484,23 @@
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -542,23 +535,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>100</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>8</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>3</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>6</v>
       </c>
       <c r="H3">
@@ -577,17 +570,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>100</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4">
         <v>10</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4">
         <v>1</v>
       </c>
       <c r="F4">
@@ -612,17 +605,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>100</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5">
         <v>8</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5">
         <v>3</v>
       </c>
       <c r="F5">
@@ -647,17 +640,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>60</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6">
         <v>7</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6">
         <v>2</v>
       </c>
       <c r="F6">
@@ -682,17 +675,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>60</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7">
         <v>7</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7">
         <v>2</v>
       </c>
       <c r="F7">
@@ -717,17 +710,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>60</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8">
         <v>7</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8">
         <v>2</v>
       </c>
       <c r="F8">
@@ -752,17 +745,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>80</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9">
         <v>5</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9">
         <v>3</v>
       </c>
       <c r="F9">
@@ -787,17 +780,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>60</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10">
         <v>7</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10">
         <v>2</v>
       </c>
       <c r="F10">
@@ -822,17 +815,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>100</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11">
         <v>5</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11">
         <v>1</v>
       </c>
       <c r="F11">
@@ -848,17 +841,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>80</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12">
         <v>5</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12">
         <v>3</v>
       </c>
       <c r="F12">
@@ -874,17 +867,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>80</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13">
         <v>5</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13">
         <v>3</v>
       </c>
       <c r="F13">
@@ -900,129 +893,129 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>100</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14">
         <v>5</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>60</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15">
         <v>7</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>80</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16">
         <v>5</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>60</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17">
         <v>7</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>100</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18">
         <v>8</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>60</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19">
         <v>7</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>60</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20">
         <v>7</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>100</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21">
         <v>8</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>100</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22">
         <v>5</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22">
         <v>1</v>
       </c>
     </row>
@@ -1041,68 +1034,68 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E106904F-8955-43C1-A89B-D5C0923EBBD3}">
   <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="R33" sqref="R33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="N2" s="1" t="s">
@@ -1118,7 +1111,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1168,7 +1161,7 @@
         <v>2.9324490000000002E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1218,7 +1211,7 @@
         <v>1.5666764E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1268,7 +1261,7 @@
         <v>1.1629967E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1318,7 +1311,7 @@
         <v>1.211039E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1368,7 +1361,7 @@
         <v>4.4111518000000002E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1418,7 +1411,7 @@
         <v>3.8608496999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1468,7 +1461,7 @@
         <v>1.4668484000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1518,7 +1511,7 @@
         <v>4.6170470999999998E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1568,7 +1561,7 @@
         <v>4.6170470999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1618,7 +1611,7 @@
         <v>4.0555139999999996E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1668,7 +1661,7 @@
         <v>7.7241949999999997E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1718,7 +1711,7 @@
         <v>7.2063371000000001E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1768,7 +1761,7 @@
         <v>4.4479633999999997E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1818,7 +1811,7 @@
         <v>3.2818470000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1868,7 +1861,7 @@
         <v>3.4003928000000003E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1918,7 +1911,7 @@
         <v>0.10737754200000001</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1968,7 +1961,7 @@
         <v>3.5813312E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2018,7 +2011,7 @@
         <v>9.7644310000000005E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2068,7 +2061,7 @@
         <v>8.4566833999999994E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2118,7 +2111,7 @@
         <v>2.9848586E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2168,7 +2161,7 @@
         <v>5.8480517000000003E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2218,7 +2211,7 @@
         <v>1.9235617E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2268,7 +2261,7 @@
         <v>4.4242542000000003E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2318,7 +2311,7 @@
         <v>4.3743402000000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2368,7 +2361,7 @@
         <v>6.4513870000000003E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2418,7 +2411,7 @@
         <v>9.0281990000000006E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2468,7 +2461,7 @@
         <v>5.8255903999999997E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2518,7 +2511,7 @@
         <v>4.3712206000000003E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2568,7 +2561,7 @@
         <v>1.6128468999999999E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2618,7 +2611,7 @@
         <v>6.0084005000000003E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2668,7 +2661,7 @@
         <v>2.2579855999999999E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2718,7 +2711,7 @@
         <v>3.3080519000000003E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2756,7 +2749,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>29</v>
       </c>

</xml_diff>